<commit_message>
fix de trucs, notament dans l'import
</commit_message>
<xml_diff>
--- a/data/cashew-sierra-leone/cashew-sierra-leone-eco.xlsx
+++ b/data/cashew-sierra-leone/cashew-sierra-leone-eco.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Study id" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="147">
   <si>
     <t xml:space="preserve">Property</t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t xml:space="preserve">Local consumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kernels Local consumption</t>
   </si>
   <si>
     <t xml:space="preserve">Regional market</t>
@@ -622,7 +625,7 @@
   </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -911,40 +914,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>2</v>
@@ -958,37 +961,37 @@
         <v>0</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1042.75341172455</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>10.0800630433094</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,37 +1002,37 @@
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,37 +1043,37 @@
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,37 +1084,37 @@
         <v>0</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>13125.0161749352</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>24.1046813654803</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1122,37 +1125,37 @@
         <v>0</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>16656.3467003473</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1163,37 +1166,37 @@
         <v>0</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>22.5001406258789</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1204,37 +1207,37 @@
         <v>527466.666666667</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1272,10 +1275,10 @@
         <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1289,10 +1292,10 @@
         <v>49</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
@@ -1306,10 +1309,10 @@
         <v>50</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>491750</v>
@@ -1323,10 +1326,10 @@
         <v>51</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>285000</v>
@@ -1340,10 +1343,10 @@
         <v>52</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>3050640</v>
@@ -1357,10 +1360,10 @@
         <v>53</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>6835400</v>
@@ -1374,10 +1377,10 @@
         <v>54</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>0</v>
@@ -1391,10 +1394,10 @@
         <v>55</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>0</v>
@@ -1408,10 +1411,10 @@
         <v>56</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>0</v>
@@ -1425,10 +1428,10 @@
         <v>57</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>0</v>
@@ -1442,10 +1445,10 @@
         <v>58</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>0</v>
@@ -1459,10 +1462,10 @@
         <v>59</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0</v>
@@ -1476,10 +1479,10 @@
         <v>49</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>838671.979878743</v>
@@ -1493,10 +1496,10 @@
         <v>50</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>245875</v>
@@ -1510,10 +1513,10 @@
         <v>51</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>27560</v>
@@ -1527,10 +1530,10 @@
         <v>52</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>3352586.01293029</v>
@@ -1544,10 +1547,10 @@
         <v>53</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>16739875</v>
@@ -1561,10 +1564,10 @@
         <v>54</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>426132</v>
@@ -1578,10 +1581,10 @@
         <v>55</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>0</v>
@@ -1595,10 +1598,10 @@
         <v>56</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>0</v>
@@ -1612,10 +1615,10 @@
         <v>57</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>0</v>
@@ -1629,10 +1632,10 @@
         <v>58</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>0</v>
@@ -1646,10 +1649,10 @@
         <v>59</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>630000</v>
@@ -1663,10 +1666,10 @@
         <v>49</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>0</v>
@@ -1680,10 +1683,10 @@
         <v>50</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>0</v>
@@ -1697,10 +1700,10 @@
         <v>51</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>0</v>
@@ -1714,10 +1717,10 @@
         <v>52</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>0</v>
@@ -1731,10 +1734,10 @@
         <v>53</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>0</v>
@@ -1748,10 +1751,10 @@
         <v>54</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>0</v>
@@ -1765,10 +1768,10 @@
         <v>55</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>0</v>
@@ -1782,10 +1785,10 @@
         <v>56</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>0</v>
@@ -1799,10 +1802,10 @@
         <v>57</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>0</v>
@@ -1816,10 +1819,10 @@
         <v>58</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>0</v>
@@ -1833,10 +1836,10 @@
         <v>59</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>0</v>
@@ -1850,10 +1853,10 @@
         <v>49</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>0</v>
@@ -1867,10 +1870,10 @@
         <v>50</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>0</v>
@@ -1884,10 +1887,10 @@
         <v>51</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>0</v>
@@ -1901,10 +1904,10 @@
         <v>52</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>0</v>
@@ -1918,10 +1921,10 @@
         <v>53</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>0</v>
@@ -1935,10 +1938,10 @@
         <v>54</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>0</v>
@@ -1952,10 +1955,10 @@
         <v>55</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>0</v>
@@ -1969,10 +1972,10 @@
         <v>56</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>0</v>
@@ -1986,10 +1989,10 @@
         <v>57</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>0</v>
@@ -2003,10 +2006,10 @@
         <v>58</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>0</v>
@@ -2020,10 +2023,10 @@
         <v>59</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>0</v>
@@ -2037,10 +2040,10 @@
         <v>49</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>5095328.02012126</v>
@@ -2054,10 +2057,10 @@
         <v>50</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>379350</v>
@@ -2071,10 +2074,10 @@
         <v>51</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>58540</v>
@@ -2088,10 +2091,10 @@
         <v>52</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>378092.487069702</v>
@@ -2105,10 +2108,10 @@
         <v>53</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>2057475</v>
@@ -2122,10 +2125,10 @@
         <v>54</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>89871</v>
@@ -2139,10 +2142,10 @@
         <v>55</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>0</v>
@@ -2156,10 +2159,10 @@
         <v>56</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>0</v>
@@ -2173,10 +2176,10 @@
         <v>57</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>0</v>
@@ -2190,10 +2193,10 @@
         <v>58</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>0</v>
@@ -2207,10 +2210,10 @@
         <v>59</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>175644</v>
@@ -2224,10 +2227,10 @@
         <v>49</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>13846000</v>
@@ -2241,10 +2244,10 @@
         <v>50</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>1545500</v>
@@ -2258,10 +2261,10 @@
         <v>51</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>409500</v>
@@ -2275,10 +2278,10 @@
         <v>52</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>7308825</v>
@@ -2292,10 +2295,10 @@
         <v>53</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>34177000</v>
@@ -2309,10 +2312,10 @@
         <v>54</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>630000</v>
@@ -2326,10 +2329,10 @@
         <v>55</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>0</v>
@@ -2343,10 +2346,10 @@
         <v>56</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>0</v>
@@ -2360,10 +2363,10 @@
         <v>57</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>0</v>
@@ -2377,10 +2380,10 @@
         <v>58</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>0</v>
@@ -2394,10 +2397,10 @@
         <v>59</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>903294</v>
@@ -2411,10 +2414,10 @@
         <v>49</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>0</v>
@@ -2428,10 +2431,10 @@
         <v>50</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>0</v>
@@ -2445,10 +2448,10 @@
         <v>51</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>0</v>
@@ -2462,10 +2465,10 @@
         <v>52</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>0</v>
@@ -2479,10 +2482,10 @@
         <v>53</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>0</v>
@@ -2496,10 +2499,10 @@
         <v>54</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E73" s="0" t="n">
         <v>0</v>
@@ -2513,10 +2516,10 @@
         <v>55</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>0</v>
@@ -2530,10 +2533,10 @@
         <v>56</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>0</v>
@@ -2547,10 +2550,10 @@
         <v>57</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>0</v>
@@ -2564,10 +2567,10 @@
         <v>58</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>0</v>
@@ -2581,10 +2584,10 @@
         <v>59</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>0</v>
@@ -2598,10 +2601,10 @@
         <v>49</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>0</v>
@@ -2615,10 +2618,10 @@
         <v>50</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>0</v>
@@ -2632,10 +2635,10 @@
         <v>51</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>0</v>
@@ -2649,10 +2652,10 @@
         <v>52</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>0</v>
@@ -2666,10 +2669,10 @@
         <v>53</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E83" s="0" t="n">
         <v>8544250</v>
@@ -2683,10 +2686,10 @@
         <v>54</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E84" s="0" t="n">
         <v>28728</v>
@@ -2700,10 +2703,10 @@
         <v>55</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>0</v>
@@ -2717,10 +2720,10 @@
         <v>56</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>0</v>
@@ -2734,10 +2737,10 @@
         <v>57</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>0</v>
@@ -2751,10 +2754,10 @@
         <v>58</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>0</v>
@@ -2768,10 +2771,10 @@
         <v>59</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E89" s="0" t="n">
         <v>97650</v>
@@ -2785,10 +2788,10 @@
         <v>49</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>7912000</v>
@@ -2802,10 +2805,10 @@
         <v>50</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E91" s="0" t="n">
         <v>428525</v>
@@ -2819,10 +2822,10 @@
         <v>51</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>38400</v>
@@ -2836,10 +2839,10 @@
         <v>52</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E93" s="0" t="n">
         <v>527506.5</v>
@@ -2853,10 +2856,10 @@
         <v>53</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>0</v>
@@ -2870,10 +2873,10 @@
         <v>54</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>12000</v>
@@ -2887,10 +2890,10 @@
         <v>55</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>0</v>
@@ -2904,10 +2907,10 @@
         <v>56</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>0</v>
@@ -2921,10 +2924,10 @@
         <v>57</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E98" s="0" t="n">
         <v>0</v>
@@ -2938,10 +2941,10 @@
         <v>58</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E99" s="0" t="n">
         <v>0</v>
@@ -2955,10 +2958,10 @@
         <v>59</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>0</v>
@@ -3255,7 +3258,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.14"/>
@@ -3263,7 +3266,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3792,8 +3795,8 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3914,7 +3917,7 @@
         <v>56</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3922,7 +3925,7 @@
         <v>57</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3930,7 +3933,7 @@
         <v>58</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3938,7 +3941,7 @@
         <v>59</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3963,7 +3966,7 @@
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.43"/>
@@ -3979,22 +3982,22 @@
         <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4194,135 +4197,135 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B2" s="9" t="n">
         <v>1113386</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B3" s="9" t="n">
         <v>26611</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B4" s="9" t="n">
         <v>25658570</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B5" s="9" t="n">
         <v>168600</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B6" s="9" t="n">
         <v>6744</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B7" s="9" t="n">
         <v>421500</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B8" s="9" t="n">
         <v>252900</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B9" s="9" t="n">
         <v>0</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B10" s="9" t="n">
         <v>0</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B11" s="9" t="n">
         <v>87923</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B12" s="9" t="n">
         <v>0</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4333,7 +4336,7 @@
         <v>35080294.0187454</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4372,13 +4375,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4460,7 +4463,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>0</v>
@@ -4468,7 +4471,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>10662790</v>
@@ -4476,7 +4479,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>8918431.5</v>
@@ -4484,7 +4487,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>0</v>
@@ -4492,7 +4495,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>8670628</v>

</xml_diff>